<commit_message>
final manuscript version, substrate testing
</commit_message>
<xml_diff>
--- a/results/tables/table_S3.xlsx
+++ b/results/tables/table_S3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters &amp; Results" sheetId="1" state="visible" r:id="rId2"/>
@@ -158,19 +158,19 @@
     <t xml:space="preserve">b0009</t>
   </si>
   <si>
+    <t xml:space="preserve">b0918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b0084</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b2557</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b4160</t>
+  </si>
+  <si>
     <t xml:space="preserve">Experimentally essential</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b0918</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b0084</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b2557</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b4160</t>
   </si>
   <si>
     <t xml:space="preserve">b3041</t>
@@ -1395,7 +1395,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1430,11 +1430,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1562,7 +1557,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1603,8 +1598,8 @@
   </sheetPr>
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F41" activeCellId="0" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1914,8 +1909,8 @@
   </sheetPr>
   <dimension ref="A1:M339"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M14" activeCellId="0" sqref="M14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2094,19 +2089,16 @@
         <v>23</v>
       </c>
       <c r="H7" s="6"/>
-      <c r="I7" s="12" t="s">
+      <c r="K7" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>44</v>
@@ -2116,7 +2108,7 @@
       </c>
       <c r="H8" s="6"/>
       <c r="K8" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2133,6 +2125,9 @@
         <v>35</v>
       </c>
       <c r="H9" s="6"/>
+      <c r="I9" s="12" t="s">
+        <v>49</v>
+      </c>
       <c r="K9" s="8" t="s">
         <v>50</v>
       </c>
@@ -2178,7 +2173,7 @@
         <v>56</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>57</v>
@@ -2217,7 +2212,7 @@
         <v>61</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>62</v>
@@ -2328,7 +2323,7 @@
         <v>69</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H20" s="6"/>
       <c r="K20" s="8" t="s">
@@ -2337,7 +2332,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>63</v>
@@ -2944,7 +2939,7 @@
       </c>
       <c r="H54" s="6"/>
       <c r="K54" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3642,7 +3637,7 @@
         <v>264</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H93" s="6"/>
       <c r="K93" s="8" t="s">
@@ -3789,7 +3784,7 @@
         <v>182</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G102" s="6" t="s">
         <v>288</v>
@@ -3861,7 +3856,7 @@
         <v>119</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D107" s="6" t="s">
         <v>72</v>

</xml_diff>